<commit_message>
updated template to final, twice now
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -776,7 +776,7 @@
   <dimension ref="A1:Z150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4773,10 +4773,10 @@
   <sheetProtection password="CC3E" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
-      <formula1>$D$13:$D$16</formula1>
+      <formula1>"S.1,S.2,S.3,S.4"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>$D$4:$D$5</formula1>
+      <formula1>"Male, Female"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
modded template for history n pol. ed
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="CC3E" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="StudentDetails" sheetId="1" r:id="rId1"/>
@@ -172,18 +172,6 @@
     <t>Geography S4</t>
   </si>
   <si>
-    <t>History S1</t>
-  </si>
-  <si>
-    <t>History S2</t>
-  </si>
-  <si>
-    <t>History S3</t>
-  </si>
-  <si>
-    <t>History S4</t>
-  </si>
-  <si>
     <t>Biology S1</t>
   </si>
   <si>
@@ -338,6 +326,18 @@
   </si>
   <si>
     <t>Topic 4</t>
+  </si>
+  <si>
+    <t>History&amp;Pol.Ed S1</t>
+  </si>
+  <si>
+    <t>History&amp;Pol.Ed S2</t>
+  </si>
+  <si>
+    <t>History&amp;Pol.Ed S3</t>
+  </si>
+  <si>
+    <t>History&amp;Pol.Ed S4</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -6113,16 +6113,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -8348,16 +8348,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -10583,16 +10583,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -12818,16 +12818,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -15053,16 +15053,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -17288,16 +17288,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -19523,16 +19523,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -21758,16 +21758,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -23993,16 +23993,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -26228,16 +26228,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -28444,8 +28444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29639,7 +29639,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -29648,7 +29648,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -29657,7 +29657,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -29666,7 +29666,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -29675,7 +29675,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -29684,7 +29684,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -29693,7 +29693,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -29702,7 +29702,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -29711,7 +29711,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -29720,7 +29720,7 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -29729,7 +29729,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -29738,7 +29738,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -29747,7 +29747,7 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -29756,7 +29756,7 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -29765,7 +29765,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -29774,7 +29774,7 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -29783,7 +29783,7 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -29792,7 +29792,7 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -29801,7 +29801,7 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -29810,7 +29810,7 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -29819,7 +29819,7 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -29828,7 +29828,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -29837,7 +29837,7 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -29846,7 +29846,7 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -29855,7 +29855,7 @@
     </row>
     <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -29864,7 +29864,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -29873,7 +29873,7 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -29882,7 +29882,7 @@
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -29891,7 +29891,7 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -29900,7 +29900,7 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -29909,7 +29909,7 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -29918,7 +29918,7 @@
     </row>
     <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -29927,7 +29927,7 @@
     </row>
     <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -29936,7 +29936,7 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -29945,7 +29945,7 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -29954,7 +29954,7 @@
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -29963,7 +29963,7 @@
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -29972,7 +29972,7 @@
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -29981,7 +29981,7 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -29990,7 +29990,7 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -29999,7 +29999,7 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -30008,7 +30008,7 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -30017,7 +30017,7 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -30026,7 +30026,7 @@
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -30035,7 +30035,7 @@
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -30044,7 +30044,7 @@
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -30053,7 +30053,7 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -30062,7 +30062,7 @@
     </row>
     <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -30071,7 +30071,7 @@
     </row>
     <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -30080,7 +30080,7 @@
     </row>
     <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -30089,7 +30089,7 @@
     </row>
     <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -30098,7 +30098,7 @@
     </row>
     <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -30139,16 +30139,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -32374,16 +32374,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -34609,16 +34609,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -36844,16 +36844,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -39079,16 +39079,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -41317,16 +41317,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -43552,16 +43552,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>